<commit_message>
g3.9b - altera ordem de exibição dos anos
</commit_message>
<xml_diff>
--- a/Data/g3.9b.xlsx
+++ b/Data/g3.9b.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2013-2024</t>
+          <t>2024-2013</t>
         </is>
       </c>
     </row>

</xml_diff>